<commit_message>
Updated the script to write the longest and shortest suggestions to Excel
</commit_message>
<xml_diff>
--- a/QUPS_keywords.xlsx
+++ b/QUPS_keywords.xlsx
@@ -40,61 +40,61 @@
     <t>keyword1</t>
   </si>
   <si>
+    <t>keyword8</t>
+  </si>
+  <si>
+    <t>keyword15</t>
+  </si>
+  <si>
     <t>keyword2</t>
   </si>
   <si>
+    <t>keyword9</t>
+  </si>
+  <si>
+    <t>keyword16</t>
+  </si>
+  <si>
     <t>keyword3</t>
   </si>
   <si>
+    <t>keyword10</t>
+  </si>
+  <si>
+    <t>keyword17</t>
+  </si>
+  <si>
     <t>keyword4</t>
   </si>
   <si>
+    <t>keyword11</t>
+  </si>
+  <si>
+    <t>keyword18</t>
+  </si>
+  <si>
     <t>keyword5</t>
   </si>
   <si>
+    <t>keyword12</t>
+  </si>
+  <si>
+    <t>keyword19</t>
+  </si>
+  <si>
     <t>keyword6</t>
   </si>
   <si>
+    <t>keyword13</t>
+  </si>
+  <si>
+    <t>keyword20</t>
+  </si>
+  <si>
     <t>keyword7</t>
   </si>
   <si>
-    <t>keyword8</t>
-  </si>
-  <si>
-    <t>keyword9</t>
-  </si>
-  <si>
-    <t>keyword10</t>
-  </si>
-  <si>
-    <t>keyword11</t>
-  </si>
-  <si>
-    <t>keyword12</t>
-  </si>
-  <si>
-    <t>keyword13</t>
-  </si>
-  <si>
     <t>keyword14</t>
-  </si>
-  <si>
-    <t>keyword15</t>
-  </si>
-  <si>
-    <t>keyword16</t>
-  </si>
-  <si>
-    <t>keyword17</t>
-  </si>
-  <si>
-    <t>keyword18</t>
-  </si>
-  <si>
-    <t>keyword19</t>
-  </si>
-  <si>
-    <t>keyword20</t>
   </si>
   <si>
     <t>keyword21</t>

</xml_diff>